<commit_message>
new ids for google sheets
</commit_message>
<xml_diff>
--- a/data/kawasaki_vehicle_config.xlsx
+++ b/data/kawasaki_vehicle_config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorgrant/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorgrant/R/kawasaki_cm360/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5DC4D314-C9DE-1246-BB79-F4CBB8A568EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A939CBB7-9F5B-4249-9E96-FECD93C67A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B7B9C377-6E49-5645-AD03-64355A1B0115}"/>
+    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{B7B9C377-6E49-5645-AD03-64355A1B0115}"/>
   </bookViews>
   <sheets>
     <sheet name="NAV" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>ID</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>cm360_report</t>
+  </si>
+  <si>
+    <t>google_sheet</t>
+  </si>
+  <si>
+    <t>1dc-SL4KNa9v89CE4lGxR1ZAdoyW1SbepHzKFf7I9__k</t>
+  </si>
+  <si>
+    <t>1ZDR9So-jv4lcPE9YTSno1Tde-xMdSHDDzReEIBmj55o</t>
   </si>
 </sst>
 </file>
@@ -417,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941A3E5D-C442-7F4C-9410-4C3BAB881AC3}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -442,6 +451,14 @@
       </c>
       <c r="B2">
         <v>1424003003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -454,10 +471,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{148C9742-60A4-E74C-8145-E6F3D7FFA3EE}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -482,6 +499,14 @@
         <v>1498754331</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
adding the ga4 path for each vehicle
</commit_message>
<xml_diff>
--- a/data/kawasaki_vehicle_config.xlsx
+++ b/data/kawasaki_vehicle_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorgrant/R/kawasaki_cm360/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082EC8D5-6AF5-2347-93A3-E4994C3E34BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AA2403-03EF-5D4E-BE05-0B83F2CAFF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B7B9C377-6E49-5645-AD03-64355A1B0115}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>1lfSZD2eR1Qozc9dkrhp2pUftvlIFmdr3Z_SyDjxNH6E</t>
+  </si>
+  <si>
+    <t>ga4_path</t>
+  </si>
+  <si>
+    <t>/en-us/nav-ptv/nav/4-passenger/nav-4e</t>
+  </si>
+  <si>
+    <t>en-us/side-x-side/teryx/teryx-4-5-passenger-supercharged/teryx4-5-h2</t>
   </si>
 </sst>
 </file>
@@ -444,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941A3E5D-C442-7F4C-9410-4C3BAB881AC3}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,6 +504,14 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
@@ -505,10 +522,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{148C9742-60A4-E74C-8145-E6F3D7FFA3EE}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,6 +574,14 @@
         <v>11</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
adding ga4 start dates
</commit_message>
<xml_diff>
--- a/data/kawasaki_vehicle_config.xlsx
+++ b/data/kawasaki_vehicle_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorgrant/R/kawasaki_cm360/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AA2403-03EF-5D4E-BE05-0B83F2CAFF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911E8E5B-E3D8-4040-8478-B8E5D742B2E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B7B9C377-6E49-5645-AD03-64355A1B0115}"/>
+    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{B7B9C377-6E49-5645-AD03-64355A1B0115}"/>
   </bookViews>
   <sheets>
     <sheet name="NAV" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>ID</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>en-us/side-x-side/teryx/teryx-4-5-passenger-supercharged/teryx4-5-h2</t>
+  </si>
+  <si>
+    <t>ga4_start</t>
   </si>
 </sst>
 </file>
@@ -117,8 +120,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941A3E5D-C442-7F4C-9410-4C3BAB881AC3}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -512,6 +516,14 @@
         <v>13</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45713</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
@@ -522,10 +534,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{148C9742-60A4-E74C-8145-E6F3D7FFA3EE}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -582,6 +594,14 @@
         <v>14</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45870</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
adding meta daily email subject
</commit_message>
<xml_diff>
--- a/data/kawasaki_vehicle_config.xlsx
+++ b/data/kawasaki_vehicle_config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorgrant/R/kawasaki_cm360/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF48FFD-65E9-5C4E-BB2F-A4BA8628E02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F1D638-97A2-3D4F-BA32-E423B5D6592F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B7B9C377-6E49-5645-AD03-64355A1B0115}"/>
+    <workbookView xWindow="1100" yWindow="760" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B7B9C377-6E49-5645-AD03-64355A1B0115}"/>
   </bookViews>
   <sheets>
     <sheet name="NAV" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>ID</t>
   </si>
@@ -94,19 +94,38 @@
   </si>
   <si>
     <t>Kawasaki 5525 Rtl Inv Daily</t>
+  </si>
+  <si>
+    <t>meta_gmail_subject</t>
+  </si>
+  <si>
+    <t>Datorama | Report "Kawasaki Daily Reporting Meta" (1159468)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Aptos Display"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,9 +148,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,10 +572,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{148C9742-60A4-E74C-8145-E6F3D7FFA3EE}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -627,6 +648,14 @@
         <v>18</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
adding a context tab describing each id
</commit_message>
<xml_diff>
--- a/data/kawasaki_vehicle_config.xlsx
+++ b/data/kawasaki_vehicle_config.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorgrant/R/kawasaki_cm360/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCC7E14-321D-1640-B579-0A8C29579B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38951111-B978-AA48-A97D-E3E7987E071C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="760" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B7B9C377-6E49-5645-AD03-64355A1B0115}"/>
+    <workbookView xWindow="1100" yWindow="760" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{B7B9C377-6E49-5645-AD03-64355A1B0115}"/>
   </bookViews>
   <sheets>
     <sheet name="NAV" sheetId="1" r:id="rId1"/>
     <sheet name="5525" sheetId="2" r:id="rId2"/>
+    <sheet name="About" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -100,6 +101,30 @@
   </si>
   <si>
     <t>Datorama | Report "Kawasaki Daily Reporting Meta" (1159468)</t>
+  </si>
+  <si>
+    <t>the report ID in CM360 for each vehicle</t>
+  </si>
+  <si>
+    <t>the workbook ID for the google sheets workbook for each vehicle</t>
+  </si>
+  <si>
+    <t>the name of the sheet used by Fuse and Looker for their dash; sheet ID is hardcoded</t>
+  </si>
+  <si>
+    <t>workbook ID for the daily Meta data that's created using datorama data</t>
+  </si>
+  <si>
+    <t>the filtered url path for each vehicle on kawi.com</t>
+  </si>
+  <si>
+    <t>the start date for which we track ga4 pageviews</t>
+  </si>
+  <si>
+    <t>the subject line of the daily sales email from kawi</t>
+  </si>
+  <si>
+    <t>the subject line of the daily meta data email from datorama</t>
   </si>
 </sst>
 </file>
@@ -490,7 +515,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection sqref="A1:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -582,7 +607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{148C9742-60A4-E74C-8145-E6F3D7FFA3EE}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -667,4 +692,91 @@
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Confidential - Not for Public Consumption or Distribution</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B33B9FD1-66F2-F643-9BE6-84DBFFD74679}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="59.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updating meta email id
</commit_message>
<xml_diff>
--- a/data/kawasaki_vehicle_config.xlsx
+++ b/data/kawasaki_vehicle_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorgrant/R/kawasaki_cm360/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8110D9-68C3-554C-8171-B4B2380011C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D6FC10-E991-3B4F-8AEB-0E309E2C5061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37700" yWindow="500" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B7B9C377-6E49-5645-AD03-64355A1B0115}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17440" xr2:uid="{B7B9C377-6E49-5645-AD03-64355A1B0115}"/>
   </bookViews>
   <sheets>
     <sheet name="NAV" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -97,9 +97,6 @@
     <t>meta_gmail_subject</t>
   </si>
   <si>
-    <t>Datorama | Report "Kawasaki Daily Reporting Meta" (1159468)</t>
-  </si>
-  <si>
     <t>the report ID in CM360 for each vehicle</t>
   </si>
   <si>
@@ -125,6 +122,9 @@
   </si>
   <si>
     <t>daily_TeryxH2</t>
+  </si>
+  <si>
+    <t>Datorama | Report "Kawasaki Daily Reporting Meta" (1161493)</t>
   </si>
 </sst>
 </file>
@@ -179,12 +179,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,7 +522,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941A3E5D-C442-7F4C-9410-4C3BAB881AC3}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -597,7 +600,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -612,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{148C9742-60A4-E74C-8145-E6F3D7FFA3EE}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -651,7 +654,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -690,7 +693,9 @@
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -723,7 +728,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -731,7 +736,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -739,7 +744,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -747,7 +752,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -755,7 +760,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -763,7 +768,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -771,7 +776,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -779,7 +784,7 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>